<commit_message>
Atualizacao - cores, limites, textos
</commit_message>
<xml_diff>
--- a/dados/dados.xlsx
+++ b/dados/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mar21\Documents\Trabalho\CGINF\Projetos_R\Servidores_por_Genero\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56D19AC-8E4B-4104-B843-6ACCF11AA6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852BCE12-F739-428C-9C44-B3D018FF10A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-4245" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="351">
   <si>
     <r>
       <t>Ano</t>
@@ -453,64 +453,19 @@
     <t>DAS-1 </t>
   </si>
   <si>
-    <t>CCE-5 </t>
-  </si>
-  <si>
-    <t>FCE-5 </t>
-  </si>
-  <si>
     <t>DAS-2 </t>
   </si>
   <si>
-    <t>CCE-7 </t>
-  </si>
-  <si>
-    <t>FCE-7 </t>
-  </si>
-  <si>
     <t>DAS-3 </t>
   </si>
   <si>
-    <t>CCE-10 </t>
-  </si>
-  <si>
-    <t>FCE-10 </t>
-  </si>
-  <si>
     <t>DAS-4 </t>
   </si>
   <si>
-    <t>CCE-13 </t>
-  </si>
-  <si>
-    <t>FCE-13 </t>
-  </si>
-  <si>
     <t>DAS-5 </t>
   </si>
   <si>
-    <t>CCE-15 </t>
-  </si>
-  <si>
-    <t>FCE-15 </t>
-  </si>
-  <si>
     <t>DAS-6 </t>
-  </si>
-  <si>
-    <t>CCE-17 </t>
-  </si>
-  <si>
-    <t>FCE-17 </t>
-  </si>
-  <si>
-    <t>NE </t>
-  </si>
-  <si>
-    <t>CCE-18 </t>
-  </si>
-  <si>
-    <t>- </t>
   </si>
   <si>
     <t>13.082 </t>
@@ -1269,15 +1224,6 @@
     <t>Homens</t>
   </si>
   <si>
-    <t>DAS</t>
-  </si>
-  <si>
-    <t>CCE</t>
-  </si>
-  <si>
-    <t>FCE</t>
-  </si>
-  <si>
     <t>Acre</t>
   </si>
   <si>
@@ -1375,6 +1321,111 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2020 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022 </t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>Nível 18</t>
+  </si>
+  <si>
+    <t>DAS/FCPE - 6</t>
+  </si>
+  <si>
+    <t>Nível 17</t>
+  </si>
+  <si>
+    <t>DAS/FCPE - 5</t>
+  </si>
+  <si>
+    <t>Nível 15 e 16</t>
+  </si>
+  <si>
+    <t>DAS/FCPE - 4</t>
+  </si>
+  <si>
+    <t>Nível 13 e 14</t>
+  </si>
+  <si>
+    <t>DAS/FCPE - 3</t>
+  </si>
+  <si>
+    <t>Nível 10 a 12</t>
+  </si>
+  <si>
+    <t>DAS/FCPE - 2</t>
+  </si>
+  <si>
+    <t>Nível 7 a 9</t>
+  </si>
+  <si>
+    <t>DAS/FCPE - 1</t>
+  </si>
+  <si>
+    <t>Nível 5 e 6</t>
+  </si>
+  <si>
+    <t>FG – 1</t>
+  </si>
+  <si>
+    <t>Nível 3 e 4</t>
+  </si>
+  <si>
+    <t>FG – 2</t>
+  </si>
+  <si>
+    <t>Nível 2</t>
+  </si>
+  <si>
+    <t>FG - 3</t>
+  </si>
+  <si>
+    <t>Nível 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nível do cargo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nível correspondente </t>
   </si>
 </sst>
 </file>
@@ -1384,7 +1435,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1417,6 +1468,12 @@
       <color rgb="FF404040"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1668,7 +1725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1760,9 +1817,12 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2341,7 +2401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{993A49C1-780E-4C27-9D18-612A9F568DFC}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2357,35 +2417,35 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="B2" s="33">
+        <v>283</v>
+      </c>
+      <c r="B2" s="32">
         <v>1468</v>
       </c>
-      <c r="C2" s="33">
+      <c r="C2" s="32">
         <v>2351</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D2" s="32">
         <f>B2+C2</f>
         <v>3819</v>
       </c>
@@ -2398,15 +2458,15 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>302</v>
-      </c>
-      <c r="B3" s="33">
+        <v>284</v>
+      </c>
+      <c r="B3" s="32">
         <v>3408</v>
       </c>
-      <c r="C3" s="33">
+      <c r="C3" s="32">
         <v>4431</v>
       </c>
-      <c r="D3" s="33">
+      <c r="D3" s="32">
         <f t="shared" ref="D3:D28" si="0">B3+C3</f>
         <v>7839</v>
       </c>
@@ -2419,15 +2479,15 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>303</v>
-      </c>
-      <c r="B4" s="33">
+        <v>285</v>
+      </c>
+      <c r="B4" s="32">
         <v>3948</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="32">
         <v>5768</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="32">
         <f t="shared" si="0"/>
         <v>9716</v>
       </c>
@@ -2440,15 +2500,15 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>304</v>
-      </c>
-      <c r="B5" s="33">
+        <v>286</v>
+      </c>
+      <c r="B5" s="32">
         <v>5156</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="32">
         <v>4775</v>
       </c>
-      <c r="D5" s="33">
+      <c r="D5" s="32">
         <f t="shared" si="0"/>
         <v>9931</v>
       </c>
@@ -2461,15 +2521,15 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="B6" s="33">
+        <v>287</v>
+      </c>
+      <c r="B6" s="32">
         <v>10174</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="32">
         <v>13329</v>
       </c>
-      <c r="D6" s="33">
+      <c r="D6" s="32">
         <f t="shared" si="0"/>
         <v>23503</v>
       </c>
@@ -2482,15 +2542,15 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>306</v>
-      </c>
-      <c r="B7" s="33">
+        <v>288</v>
+      </c>
+      <c r="B7" s="32">
         <v>7342</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="32">
         <v>10462</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="32">
         <f t="shared" si="0"/>
         <v>17804</v>
       </c>
@@ -2503,15 +2563,15 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>307</v>
-      </c>
-      <c r="B8" s="33">
+        <v>289</v>
+      </c>
+      <c r="B8" s="32">
         <v>34246</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="32">
         <v>43463</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="32">
         <f t="shared" si="0"/>
         <v>77709</v>
       </c>
@@ -2524,15 +2584,15 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>308</v>
-      </c>
-      <c r="B9" s="33">
+        <v>290</v>
+      </c>
+      <c r="B9" s="32">
         <v>4161</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="32">
         <v>6081</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="32">
         <f t="shared" si="0"/>
         <v>10242</v>
       </c>
@@ -2545,15 +2605,15 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>309</v>
-      </c>
-      <c r="B10" s="33">
+        <v>291</v>
+      </c>
+      <c r="B10" s="32">
         <v>6141</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="32">
         <v>7377</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="32">
         <f t="shared" si="0"/>
         <v>13518</v>
       </c>
@@ -2566,15 +2626,15 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
-        <v>310</v>
-      </c>
-      <c r="B11" s="33">
+        <v>292</v>
+      </c>
+      <c r="B11" s="32">
         <v>4864</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="32">
         <v>6974</v>
       </c>
-      <c r="D11" s="33">
+      <c r="D11" s="32">
         <f t="shared" si="0"/>
         <v>11838</v>
       </c>
@@ -2587,15 +2647,15 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
-        <v>311</v>
-      </c>
-      <c r="B12" s="33">
+        <v>293</v>
+      </c>
+      <c r="B12" s="32">
         <v>23517</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="32">
         <v>28406</v>
       </c>
-      <c r="D12" s="33">
+      <c r="D12" s="32">
         <f t="shared" si="0"/>
         <v>51923</v>
       </c>
@@ -2608,15 +2668,15 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
-        <v>312</v>
-      </c>
-      <c r="B13" s="33">
+        <v>294</v>
+      </c>
+      <c r="B13" s="32">
         <v>4164</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="32">
         <v>6106</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="32">
         <f t="shared" si="0"/>
         <v>10270</v>
       </c>
@@ -2629,15 +2689,15 @@
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
-        <v>313</v>
-      </c>
-      <c r="B14" s="33">
+        <v>295</v>
+      </c>
+      <c r="B14" s="32">
         <v>3715</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="32">
         <v>5108</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D14" s="32">
         <f t="shared" si="0"/>
         <v>8823</v>
       </c>
@@ -2650,15 +2710,15 @@
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="B15" s="33">
+        <v>296</v>
+      </c>
+      <c r="B15" s="32">
         <v>7613</v>
       </c>
-      <c r="C15" s="33">
+      <c r="C15" s="32">
         <v>10871</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D15" s="32">
         <f t="shared" si="0"/>
         <v>18484</v>
       </c>
@@ -2671,15 +2731,15 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
-        <v>315</v>
-      </c>
-      <c r="B16" s="33">
+        <v>297</v>
+      </c>
+      <c r="B16" s="32">
         <v>6680</v>
       </c>
-      <c r="C16" s="33">
+      <c r="C16" s="32">
         <v>8564</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D16" s="32">
         <f t="shared" si="0"/>
         <v>15244</v>
       </c>
@@ -2692,15 +2752,15 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>316</v>
-      </c>
-      <c r="B17" s="33">
+        <v>298</v>
+      </c>
+      <c r="B17" s="32">
         <v>9598</v>
       </c>
-      <c r="C17" s="33">
+      <c r="C17" s="32">
         <v>12624</v>
       </c>
-      <c r="D17" s="33">
+      <c r="D17" s="32">
         <f t="shared" si="0"/>
         <v>22222</v>
       </c>
@@ -2713,15 +2773,15 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>317</v>
-      </c>
-      <c r="B18" s="33">
+        <v>299</v>
+      </c>
+      <c r="B18" s="32">
         <v>3551</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C18" s="32">
         <v>5205</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="32">
         <f t="shared" si="0"/>
         <v>8756</v>
       </c>
@@ -2734,15 +2794,15 @@
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
-        <v>318</v>
-      </c>
-      <c r="B19" s="33">
+        <v>300</v>
+      </c>
+      <c r="B19" s="32">
         <v>9536</v>
       </c>
-      <c r="C19" s="33">
+      <c r="C19" s="32">
         <v>12534</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="32">
         <f t="shared" si="0"/>
         <v>22070</v>
       </c>
@@ -2755,15 +2815,15 @@
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>319</v>
-      </c>
-      <c r="B20" s="33">
+        <v>301</v>
+      </c>
+      <c r="B20" s="32">
         <v>44645</v>
       </c>
-      <c r="C20" s="33">
+      <c r="C20" s="32">
         <v>44698</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="32">
         <f t="shared" si="0"/>
         <v>89343</v>
       </c>
@@ -2776,15 +2836,15 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>320</v>
-      </c>
-      <c r="B21" s="33">
+        <v>302</v>
+      </c>
+      <c r="B21" s="32">
         <v>5537</v>
       </c>
-      <c r="C21" s="33">
+      <c r="C21" s="32">
         <v>8191</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="32">
         <f t="shared" si="0"/>
         <v>13728</v>
       </c>
@@ -2797,15 +2857,15 @@
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="B22" s="33">
+        <v>303</v>
+      </c>
+      <c r="B22" s="32">
         <v>5314</v>
       </c>
-      <c r="C22" s="33">
+      <c r="C22" s="32">
         <v>6057</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="32">
         <f t="shared" si="0"/>
         <v>11371</v>
       </c>
@@ -2818,15 +2878,15 @@
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>322</v>
-      </c>
-      <c r="B23" s="33">
+        <v>304</v>
+      </c>
+      <c r="B23" s="32">
         <v>3705</v>
       </c>
-      <c r="C23" s="33">
+      <c r="C23" s="32">
         <v>3570</v>
       </c>
-      <c r="D23" s="33">
+      <c r="D23" s="32">
         <f t="shared" si="0"/>
         <v>7275</v>
       </c>
@@ -2839,15 +2899,15 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>323</v>
-      </c>
-      <c r="B24" s="33">
+        <v>305</v>
+      </c>
+      <c r="B24" s="32">
         <v>15793</v>
       </c>
-      <c r="C24" s="33">
+      <c r="C24" s="32">
         <v>17410</v>
       </c>
-      <c r="D24" s="33">
+      <c r="D24" s="32">
         <f t="shared" si="0"/>
         <v>33203</v>
       </c>
@@ -2860,15 +2920,15 @@
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
-        <v>324</v>
-      </c>
-      <c r="B25" s="33">
+        <v>306</v>
+      </c>
+      <c r="B25" s="32">
         <v>7522</v>
       </c>
-      <c r="C25" s="33">
+      <c r="C25" s="32">
         <v>9625</v>
       </c>
-      <c r="D25" s="33">
+      <c r="D25" s="32">
         <f t="shared" si="0"/>
         <v>17147</v>
       </c>
@@ -2881,15 +2941,15 @@
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="B26" s="33">
+        <v>307</v>
+      </c>
+      <c r="B26" s="32">
         <v>2818</v>
       </c>
-      <c r="C26" s="33">
+      <c r="C26" s="32">
         <v>3651</v>
       </c>
-      <c r="D26" s="33">
+      <c r="D26" s="32">
         <f t="shared" si="0"/>
         <v>6469</v>
       </c>
@@ -2902,15 +2962,15 @@
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
-        <v>326</v>
-      </c>
-      <c r="B27" s="33">
+        <v>308</v>
+      </c>
+      <c r="B27" s="32">
         <v>16579</v>
       </c>
-      <c r="C27" s="33">
+      <c r="C27" s="32">
         <v>21167</v>
       </c>
-      <c r="D27" s="33">
+      <c r="D27" s="32">
         <f t="shared" si="0"/>
         <v>37746</v>
       </c>
@@ -2923,15 +2983,15 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="B28" s="33">
+        <v>309</v>
+      </c>
+      <c r="B28" s="32">
         <v>2078</v>
       </c>
-      <c r="C28" s="33">
+      <c r="C28" s="32">
         <v>2937</v>
       </c>
-      <c r="D28" s="33">
+      <c r="D28" s="32">
         <f t="shared" si="0"/>
         <v>5015</v>
       </c>
@@ -2950,100 +3010,104 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E265F76-9428-4140-B6CC-0CC20C584D43}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="87.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>329</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>331</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>333</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>335</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>337</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>339</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>341</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" t="s">
-        <v>122</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>343</v>
+      </c>
+      <c r="B9" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>345</v>
+      </c>
+      <c r="B10" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>347</v>
+      </c>
+      <c r="B11" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -3076,22 +3140,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C1" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="E1" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="F1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3099,13 +3163,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
         <v>91</v>
@@ -3119,13 +3183,13 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="E3" t="s">
         <v>96</v>
@@ -3139,19 +3203,19 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="F4" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3159,19 +3223,19 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="F5" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3179,13 +3243,13 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E6" t="s">
         <v>91</v>
@@ -3199,19 +3263,19 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="F7" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3219,19 +3283,19 @@
         <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="E8" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="F8" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3239,19 +3303,19 @@
         <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="E9" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="F9" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3259,19 +3323,19 @@
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="E10" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="F10" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3279,19 +3343,19 @@
         <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="D11" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F11" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3299,19 +3363,19 @@
         <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D12" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="E12" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="F12" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3319,19 +3383,19 @@
         <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C13" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D13" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="E13" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="F13" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3351,22 +3415,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C1" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="E1" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="F1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3374,13 +3438,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
         <v>91</v>
@@ -3394,13 +3458,13 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="E3" t="s">
         <v>96</v>
@@ -3414,19 +3478,19 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="F4" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3434,19 +3498,19 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="F5" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3454,13 +3518,13 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E6" t="s">
         <v>91</v>
@@ -3474,19 +3538,19 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="F7" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3494,19 +3558,19 @@
         <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="C8" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="E8" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="F8" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3514,19 +3578,19 @@
         <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="E9" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="F9" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3534,19 +3598,19 @@
         <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="D10" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="E10" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="F10" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3554,19 +3618,19 @@
         <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="D11" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="F11" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3574,19 +3638,19 @@
         <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C12" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D12" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="E12" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="F12" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3594,19 +3658,19 @@
         <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C13" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="D13" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="E13" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="F13" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -3629,323 +3693,323 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>102</v>
       </c>
       <c r="D1" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>111</v>
-      </c>
       <c r="G1" s="22" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>75</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>95</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>95</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>83</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>80</v>
@@ -3954,27 +4018,27 @@
         <v>93</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>81</v>
@@ -3983,22 +4047,22 @@
         <v>94</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -4036,7 +4100,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4047,10 +4111,10 @@
         <v>25089</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>87</v>
@@ -4059,7 +4123,7 @@
         <v>88</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4067,13 +4131,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>40</v>
@@ -4082,7 +4146,7 @@
         <v>41</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4090,13 +4154,13 @@
         <v>18</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="C4" s="27">
         <v>31698</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>87</v>
@@ -4105,7 +4169,7 @@
         <v>88</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4113,13 +4177,13 @@
         <v>24</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>22</v>
@@ -4128,7 +4192,7 @@
         <v>23</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4136,22 +4200,22 @@
         <v>30</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4159,22 +4223,22 @@
         <v>36</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4182,13 +4246,13 @@
         <v>42</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>98</v>
@@ -4197,7 +4261,7 @@
         <v>99</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4205,13 +4269,13 @@
         <v>48</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>93</v>
@@ -4220,7 +4284,7 @@
         <v>94</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4228,13 +4292,13 @@
         <v>54</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>93</v>
@@ -4243,7 +4307,7 @@
         <v>94</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4251,13 +4315,13 @@
         <v>60</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>89</v>
@@ -4266,7 +4330,7 @@
         <v>90</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4274,13 +4338,13 @@
         <v>66</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>100</v>
@@ -4289,7 +4353,7 @@
         <v>101</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -4297,13 +4361,13 @@
         <v>70</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>85</v>
@@ -4312,7 +4376,7 @@
         <v>86</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -4326,7 +4390,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4338,13 +4402,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="B1" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="C1" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -4354,253 +4418,254 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="31">
-        <v>40179</v>
-      </c>
-      <c r="B2" s="32">
+      <c r="A2" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="B2" s="31">
         <v>258174</v>
       </c>
-      <c r="C2" s="32">
+      <c r="C2" s="31">
         <v>322178</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="31">
         <f>B2/SUM(B2:C2)</f>
         <v>0.44485760366122629</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="31">
         <f>C2/SUM(B2:C2)</f>
         <v>0.55514239633877371</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="31">
-        <v>40544</v>
-      </c>
-      <c r="B3" s="32">
+      <c r="A3" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="B3" s="31">
         <v>261352</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="31">
         <v>323767</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="31">
         <f t="shared" ref="D3:D14" si="0">B3/SUM(B3:C3)</f>
         <v>0.44666469555765581</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="31">
         <f t="shared" ref="E3:E14" si="1">C3/SUM(B3:C3)</f>
         <v>0.55333530444234424</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="31">
-        <v>40909</v>
-      </c>
-      <c r="B4" s="32">
+      <c r="A4" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="B4" s="31">
         <v>264678</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="31">
         <v>326165</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <f t="shared" si="0"/>
         <v>0.44796671873915744</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="31">
         <f t="shared" si="1"/>
         <v>0.55203328126084261</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="31">
-        <v>41275</v>
-      </c>
-      <c r="B5" s="32">
+      <c r="A5" s="33" t="s">
+        <v>319</v>
+      </c>
+      <c r="B5" s="31">
         <v>271661</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="31">
         <v>331034</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="31">
         <f t="shared" si="0"/>
         <v>0.45074374268908818</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="31">
         <f t="shared" si="1"/>
         <v>0.54925625731091177</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="31">
-        <v>41640</v>
-      </c>
-      <c r="B6" s="32">
+      <c r="A6" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="B6" s="31">
         <v>282372</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="31">
         <v>341723</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <f t="shared" si="0"/>
         <v>0.45245034810405466</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="31">
         <f t="shared" si="1"/>
         <v>0.54754965189594529</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
-        <v>42005</v>
-      </c>
-      <c r="B7" s="32">
+      <c r="A7" s="33" t="s">
+        <v>321</v>
+      </c>
+      <c r="B7" s="31">
         <v>285186</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="31">
         <v>342241</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="31">
         <f t="shared" si="0"/>
         <v>0.45453255916624563</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="31">
         <f t="shared" si="1"/>
         <v>0.54546744083375431</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="31">
-        <v>42370</v>
-      </c>
-      <c r="B8" s="32">
+      <c r="A8" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="B8" s="31">
         <v>288289</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="31">
         <v>344196</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <f t="shared" si="0"/>
         <v>0.45580369494928735</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <f t="shared" si="1"/>
         <v>0.5441963050507127</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
-        <v>42736</v>
-      </c>
-      <c r="B9" s="32">
+      <c r="A9" s="33" t="s">
+        <v>323</v>
+      </c>
+      <c r="B9" s="31">
         <v>289675</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="31">
         <v>344482</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <f t="shared" si="0"/>
         <v>0.45678751476369417</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="31">
         <f t="shared" si="1"/>
         <v>0.54321248523630583</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="31">
-        <v>43101</v>
-      </c>
-      <c r="B10" s="32">
+      <c r="A10" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="B10" s="31">
         <v>289388</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>341301</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <f t="shared" si="0"/>
         <v>0.45884421640459877</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <f t="shared" si="1"/>
         <v>0.54115578359540117</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="31">
-        <v>43466</v>
-      </c>
-      <c r="B11" s="32">
+      <c r="A11" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="B11" s="31">
         <v>278395</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="31">
         <v>329438</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="31">
         <f t="shared" si="0"/>
         <v>0.45801231588281649</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="31">
         <f t="shared" si="1"/>
         <v>0.54198768411718345</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="31">
-        <v>43831</v>
-      </c>
-      <c r="B12" s="32">
+      <c r="A12" s="33" t="s">
+        <v>326</v>
+      </c>
+      <c r="B12" s="31">
         <v>273748</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="31">
         <v>326104</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="31">
         <f t="shared" si="0"/>
         <v>0.45635923527803524</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <f t="shared" si="1"/>
         <v>0.54364076472196476</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="31">
-        <v>44197</v>
-      </c>
-      <c r="B13" s="32">
+      <c r="A13" s="33" t="s">
+        <v>327</v>
+      </c>
+      <c r="B13" s="31">
         <v>264387</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="31">
         <v>319287</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="31">
         <f t="shared" si="0"/>
         <v>0.45297032247453201</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="31">
         <f t="shared" si="1"/>
         <v>0.54702967752546794</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="31">
-        <v>44562</v>
-      </c>
-      <c r="B14" s="32">
+      <c r="A14" s="33" t="s">
+        <v>328</v>
+      </c>
+      <c r="B14" s="31">
         <v>253264</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="31">
         <v>311735</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="31">
         <f t="shared" si="0"/>
         <v>0.44825566062948785</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="31">
         <f t="shared" si="1"/>
         <v>0.55174433937051215</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>